<commit_message>
Tested all primary matches
</commit_message>
<xml_diff>
--- a/src/test/resources/simplePairMatching.xlsx
+++ b/src/test/resources/simplePairMatching.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Java\roommateMatching\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F06615-7AF7-4A8D-A02F-8999151162E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD6E5B8-2ED9-4AA5-84F9-87BDE2CA4B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t>Id</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Mia Santos</t>
+  </si>
+  <si>
+    <t>anonymous</t>
   </si>
 </sst>
 </file>
@@ -966,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -975,7 +978,7 @@
     <col min="1" max="25" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1068,8 +1071,18 @@
       </c>
     </row>
     <row r="2" spans="1:30" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45067.989583333336</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45067.990972222222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="6" t="s">
         <v>36</v>
@@ -1148,8 +1161,18 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45069.840277777781</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45069.842361111114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="F3" s="6" t="s">
         <v>41</v>
@@ -1228,8 +1251,18 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45071.589583333334</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45071.592361111114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="6" t="s">
         <v>44</v>
@@ -1308,8 +1341,18 @@
       </c>
     </row>
     <row r="5" spans="1:30" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45071.646527777775</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45071.648611111108</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="6" t="s">
         <v>48</v>
@@ -1388,8 +1431,18 @@
       </c>
     </row>
     <row r="6" spans="1:30" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45071.915277777778</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45071.919444444444</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="6" t="s">
         <v>58</v>
@@ -1468,8 +1521,18 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.75">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45072.915277777778</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45072.919444444444</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
       <c r="F7" s="6" t="s">
         <v>60</v>
       </c>

</xml_diff>